<commit_message>
split N7-S5 barcodes into MiSeq and HiSeq
</commit_message>
<xml_diff>
--- a/barcodes/data/barcodes.xlsx
+++ b/barcodes/data/barcodes.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24580" windowHeight="23120" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="S5-N7" sheetId="1" r:id="rId1"/>
-    <sheet name="515FB" sheetId="2" r:id="rId2"/>
+    <sheet name="S5-N7_HiSeq" sheetId="3" r:id="rId1"/>
+    <sheet name="S5-N7_MiSeq" sheetId="1" r:id="rId2"/>
+    <sheet name="515FB" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" iterateCount="1" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5531" uniqueCount="3514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5776" uniqueCount="3538">
   <si>
     <t>sequence</t>
   </si>
@@ -10570,6 +10571,78 @@
   </si>
   <si>
     <t>CGATCAGT</t>
+  </si>
+  <si>
+    <t>GCGATCTA</t>
+  </si>
+  <si>
+    <t>ATAGAGAG</t>
+  </si>
+  <si>
+    <t>AGAGGATA</t>
+  </si>
+  <si>
+    <t>TCTACTCT</t>
+  </si>
+  <si>
+    <t>CTCCTTAC</t>
+  </si>
+  <si>
+    <t>TATGCAGT</t>
+  </si>
+  <si>
+    <t>TACTCCTT</t>
+  </si>
+  <si>
+    <t>AGGCTTAG</t>
+  </si>
+  <si>
+    <t>GAGTAGCC</t>
+  </si>
+  <si>
+    <t>GTCTGAGG</t>
+  </si>
+  <si>
+    <t>CGTAAGGA</t>
+  </si>
+  <si>
+    <t>CCACGCGT</t>
+  </si>
+  <si>
+    <t>GGAGTTCC</t>
+  </si>
+  <si>
+    <t>CATGGCCA</t>
+  </si>
+  <si>
+    <t>AATCTCTC</t>
+  </si>
+  <si>
+    <t>TAACCGCG</t>
+  </si>
+  <si>
+    <t>TGGCGGTC</t>
+  </si>
+  <si>
+    <t>CCATCTTA</t>
+  </si>
+  <si>
+    <t>ATGTCAAT</t>
+  </si>
+  <si>
+    <t>AGTTGGCT</t>
+  </si>
+  <si>
+    <t>ACCTAGTA</t>
+  </si>
+  <si>
+    <t>AACCGTGA</t>
+  </si>
+  <si>
+    <t>TCATTACA</t>
+  </si>
+  <si>
+    <t>CTGACGTG</t>
   </si>
 </sst>
 </file>
@@ -10886,8 +10959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11325,7 +11398,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>3514</v>
       </c>
       <c r="C26" t="s">
         <v>51</v>
@@ -11342,7 +11415,7 @@
         <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>3515</v>
       </c>
       <c r="C27" t="s">
         <v>54</v>
@@ -11359,7 +11432,7 @@
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>3516</v>
       </c>
       <c r="C28" t="s">
         <v>57</v>
@@ -11376,7 +11449,7 @@
         <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>3517</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
@@ -11393,7 +11466,7 @@
         <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>3518</v>
       </c>
       <c r="C30" t="s">
         <v>63</v>
@@ -11410,7 +11483,7 @@
         <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>3519</v>
       </c>
       <c r="C31" t="s">
         <v>66</v>
@@ -11427,7 +11500,7 @@
         <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>3520</v>
       </c>
       <c r="C32" t="s">
         <v>69</v>
@@ -11444,7 +11517,7 @@
         <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>3521</v>
       </c>
       <c r="C33" t="s">
         <v>72</v>
@@ -11461,7 +11534,7 @@
         <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>3522</v>
       </c>
       <c r="C34" t="s">
         <v>75</v>
@@ -11478,7 +11551,7 @@
         <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>3523</v>
       </c>
       <c r="C35" t="s">
         <v>78</v>
@@ -11495,7 +11568,7 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>3524</v>
       </c>
       <c r="C36" t="s">
         <v>81</v>
@@ -11512,7 +11585,7 @@
         <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>3525</v>
       </c>
       <c r="C37" t="s">
         <v>84</v>
@@ -11529,7 +11602,7 @@
         <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>3526</v>
       </c>
       <c r="C38" t="s">
         <v>87</v>
@@ -11546,7 +11619,7 @@
         <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>3527</v>
       </c>
       <c r="C39" t="s">
         <v>90</v>
@@ -11563,7 +11636,7 @@
         <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>3528</v>
       </c>
       <c r="C40" t="s">
         <v>93</v>
@@ -11580,7 +11653,7 @@
         <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>3529</v>
       </c>
       <c r="C41" t="s">
         <v>96</v>
@@ -11597,7 +11670,7 @@
         <v>98</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>3530</v>
       </c>
       <c r="C42" t="s">
         <v>99</v>
@@ -11614,7 +11687,7 @@
         <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>3531</v>
       </c>
       <c r="C43" t="s">
         <v>102</v>
@@ -11631,7 +11704,7 @@
         <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>3532</v>
       </c>
       <c r="C44" t="s">
         <v>105</v>
@@ -11648,7 +11721,7 @@
         <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>3533</v>
       </c>
       <c r="C45" t="s">
         <v>108</v>
@@ -11665,7 +11738,7 @@
         <v>110</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>3534</v>
       </c>
       <c r="C46" t="s">
         <v>111</v>
@@ -11682,7 +11755,7 @@
         <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>3535</v>
       </c>
       <c r="C47" t="s">
         <v>114</v>
@@ -11699,7 +11772,7 @@
         <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>3536</v>
       </c>
       <c r="C48" t="s">
         <v>117</v>
@@ -11716,7 +11789,7 @@
         <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>3537</v>
       </c>
       <c r="C49" t="s">
         <v>120</v>
@@ -11734,6 +11807,857 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="66.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3488</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3490</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3491</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3492</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3493</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3494</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3495</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3496</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3497</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3498</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3499</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3502</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3504</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3505</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3506</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3507</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3508</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3511</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3512</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3513</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s">
+        <v>125</v>
+      </c>
+      <c r="E47" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" t="s">
+        <v>125</v>
+      </c>
+      <c r="E48" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" t="s">
+        <v>125</v>
+      </c>
+      <c r="E49" t="s">
+        <v>312</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1057"/>
   <sheetViews>

</xml_diff>

<commit_message>
flipped N7 & S5 barcodes; fixed index2well bug
</commit_message>
<xml_diff>
--- a/barcodes/data/barcodes.xlsx
+++ b/barcodes/data/barcodes.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="240" yWindow="460" windowWidth="24580" windowHeight="23120" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="S5-N7_HiSeq" sheetId="3" r:id="rId1"/>
-    <sheet name="S5-N7_MiSeq" sheetId="1" r:id="rId2"/>
+    <sheet name="N7-S5_HiSeq" sheetId="3" r:id="rId1"/>
+    <sheet name="N7-S5_MiSeq" sheetId="1" r:id="rId2"/>
     <sheet name="515FB" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" iterateCount="1" concurrentCalc="0"/>
@@ -10960,7 +10960,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10996,10 +10996,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -11013,10 +11013,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E3" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -11030,10 +11030,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -11047,10 +11047,10 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -11064,10 +11064,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -11081,10 +11081,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E7" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -11098,10 +11098,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -11115,10 +11115,10 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E9" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -11132,10 +11132,10 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E10" t="s">
-        <v>3486</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -11149,10 +11149,10 @@
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
-        <v>3486</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -11166,10 +11166,10 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E12" t="s">
-        <v>3486</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -11183,10 +11183,10 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
-        <v>3486</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -11200,10 +11200,10 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E14" t="s">
-        <v>3487</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -11217,10 +11217,10 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
-        <v>3487</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -11234,10 +11234,10 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E16" t="s">
-        <v>3487</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -11251,10 +11251,10 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E17" t="s">
-        <v>3487</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -11268,10 +11268,10 @@
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E18" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -11285,10 +11285,10 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E19" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -11302,10 +11302,10 @@
         <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E20" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -11319,10 +11319,10 @@
         <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -11336,10 +11336,10 @@
         <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E22" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -11353,10 +11353,10 @@
         <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -11370,10 +11370,10 @@
         <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E24" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -11387,10 +11387,10 @@
         <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E25" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -11404,10 +11404,10 @@
         <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -11421,10 +11421,10 @@
         <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -11438,10 +11438,10 @@
         <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -11455,10 +11455,10 @@
         <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E29" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -11472,10 +11472,10 @@
         <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E30" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -11489,10 +11489,10 @@
         <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -11506,10 +11506,10 @@
         <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E32" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -11523,10 +11523,10 @@
         <v>72</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E33" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -11540,10 +11540,10 @@
         <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E34" t="s">
-        <v>309</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -11557,10 +11557,10 @@
         <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E35" t="s">
-        <v>309</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -11574,10 +11574,10 @@
         <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E36" t="s">
-        <v>309</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -11591,10 +11591,10 @@
         <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E37" t="s">
-        <v>309</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -11608,10 +11608,10 @@
         <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E38" t="s">
-        <v>309</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -11625,10 +11625,10 @@
         <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E39" t="s">
-        <v>309</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -11642,10 +11642,10 @@
         <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E40" t="s">
-        <v>309</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -11659,10 +11659,10 @@
         <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E41" t="s">
-        <v>309</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -11676,10 +11676,10 @@
         <v>99</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E42" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -11693,10 +11693,10 @@
         <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E43" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -11710,10 +11710,10 @@
         <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E44" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -11727,10 +11727,10 @@
         <v>108</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E45" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -11744,10 +11744,10 @@
         <v>111</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E46" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -11761,10 +11761,10 @@
         <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -11778,10 +11778,10 @@
         <v>117</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E48" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -11795,10 +11795,10 @@
         <v>120</v>
       </c>
       <c r="D49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E49" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
   </sheetData>
@@ -11811,7 +11811,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11847,10 +11847,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -11864,10 +11864,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E3" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -11881,10 +11881,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -11898,10 +11898,10 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -11915,10 +11915,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -11932,10 +11932,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E7" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -11949,10 +11949,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -11966,10 +11966,10 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E9" t="s">
-        <v>3486</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -11983,10 +11983,10 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E10" t="s">
-        <v>3486</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -12000,10 +12000,10 @@
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
-        <v>3486</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -12017,10 +12017,10 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E12" t="s">
-        <v>3486</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -12034,10 +12034,10 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
-        <v>3486</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -12051,10 +12051,10 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E14" t="s">
-        <v>3487</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -12068,10 +12068,10 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
-        <v>3487</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -12085,10 +12085,10 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E16" t="s">
-        <v>3487</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -12102,10 +12102,10 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E17" t="s">
-        <v>3487</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -12119,10 +12119,10 @@
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E18" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -12136,10 +12136,10 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E19" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -12153,10 +12153,10 @@
         <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E20" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -12170,10 +12170,10 @@
         <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -12187,10 +12187,10 @@
         <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E22" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -12204,10 +12204,10 @@
         <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -12221,10 +12221,10 @@
         <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E24" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -12238,10 +12238,10 @@
         <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E25" t="s">
-        <v>3487</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -12255,10 +12255,10 @@
         <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -12272,10 +12272,10 @@
         <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -12289,10 +12289,10 @@
         <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -12306,10 +12306,10 @@
         <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E29" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -12323,10 +12323,10 @@
         <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E30" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -12340,10 +12340,10 @@
         <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -12357,10 +12357,10 @@
         <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E32" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -12374,10 +12374,10 @@
         <v>72</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E33" t="s">
-        <v>306</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -12391,10 +12391,10 @@
         <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E34" t="s">
-        <v>309</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -12408,10 +12408,10 @@
         <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E35" t="s">
-        <v>309</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -12425,10 +12425,10 @@
         <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E36" t="s">
-        <v>309</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -12442,10 +12442,10 @@
         <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E37" t="s">
-        <v>309</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -12459,10 +12459,10 @@
         <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E38" t="s">
-        <v>309</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -12476,10 +12476,10 @@
         <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E39" t="s">
-        <v>309</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -12493,10 +12493,10 @@
         <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E40" t="s">
-        <v>309</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -12510,10 +12510,10 @@
         <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E41" t="s">
-        <v>309</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -12527,10 +12527,10 @@
         <v>99</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E42" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -12544,10 +12544,10 @@
         <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E43" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -12561,10 +12561,10 @@
         <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E44" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -12578,10 +12578,10 @@
         <v>108</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E45" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -12595,10 +12595,10 @@
         <v>111</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E46" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -12612,10 +12612,10 @@
         <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -12629,10 +12629,10 @@
         <v>117</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E48" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -12646,10 +12646,10 @@
         <v>120</v>
       </c>
       <c r="D49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E49" t="s">
-        <v>312</v>
+        <v>3487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>